<commit_message>
added invoices controllers, routes and validators and providers's funcions
</commit_message>
<xml_diff>
--- a/src/docs/AVANCES Y ESTADO CAFESENA.xlsx
+++ b/src/docs/AVANCES Y ESTADO CAFESENA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\CAFESENA\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F74512A-1313-40A3-9F8A-951750B457CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95E741FF-0C5C-44F1-909E-831174C00663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7800380C-F8C6-4977-A790-CAF0C5D5273B}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="79">
   <si>
     <t>Categorias</t>
   </si>
@@ -246,7 +245,7 @@
     <t>http://localhost:3000/api/v1/details/create</t>
   </si>
   <si>
-    <t>facturas</t>
+    <t>Facturas</t>
   </si>
   <si>
     <t>http://localhost:3000/api/v1/invoices</t>
@@ -255,13 +254,25 @@
     <t>http://localhost:3000/api/v1/invoices/1</t>
   </si>
   <si>
-    <t>http://localhost:3000/api/v1/invoices/users/erxyjd1aclv5t60t8</t>
+    <t>http://localhost:3000/api/v1/invoices/create</t>
   </si>
   <si>
     <t>http://localhost:3000/api/v1/invoices/update/1</t>
   </si>
   <si>
-    <t>http://localhost:3000/api/v1/invoices/create</t>
+    <t>Proveedores-productos</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/v1/products/providers/erxyjd754lv79fa6s</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/v1/providers/products/erxyjd92wlv86v4x0</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/v1/providers/products/create</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/v1/providers/products/update/1</t>
   </si>
 </sst>
 </file>
@@ -406,14 +417,14 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DB534A-6EEF-404A-859F-51AFC01E497C}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,22 +783,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11">
+      <c r="A1" s="13">
         <v>44669</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -819,7 +830,7 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -836,7 +847,7 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -851,7 +862,7 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -866,7 +877,7 @@
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -879,25 +890,25 @@
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="13">
         <v>44669</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -929,7 +940,7 @@
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -946,7 +957,7 @@
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -961,7 +972,7 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -976,7 +987,7 @@
       <c r="D16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -991,7 +1002,7 @@
       <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -1006,7 +1017,7 @@
       <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -1021,7 +1032,7 @@
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -1030,25 +1041,25 @@
       <c r="B20" s="4"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="13">
         <v>44669</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1080,7 +1091,7 @@
       <c r="D25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1097,7 +1108,7 @@
       <c r="D26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -1112,7 +1123,7 @@
       <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -1127,7 +1138,7 @@
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
@@ -1142,7 +1153,7 @@
       <c r="D29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -1151,25 +1162,25 @@
       <c r="B30" s="4"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="13">
         <v>44669</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1201,7 +1212,7 @@
       <c r="D35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1218,7 +1229,7 @@
       <c r="D36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -1233,7 +1244,7 @@
       <c r="D37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="13"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
@@ -1248,7 +1259,7 @@
       <c r="D38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="13"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
@@ -1257,25 +1268,25 @@
       <c r="B39" s="4"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="13"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="A41" s="13">
         <v>44699</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1307,7 +1318,7 @@
       <c r="D44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E44" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1324,7 +1335,7 @@
       <c r="D45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="13"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1339,7 +1350,7 @@
       <c r="D46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
@@ -1354,7 +1365,7 @@
       <c r="D47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -1363,25 +1374,25 @@
       <c r="B48" s="4"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="13"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="A50" s="13">
         <v>44699</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -1413,7 +1424,7 @@
       <c r="D53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1430,7 +1441,7 @@
       <c r="D54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="13"/>
+      <c r="E54" s="12"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
@@ -1445,7 +1456,7 @@
       <c r="D55" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="13"/>
+      <c r="E55" s="12"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
@@ -1460,7 +1471,7 @@
       <c r="D56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E56" s="13"/>
+      <c r="E56" s="12"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -1469,25 +1480,25 @@
       <c r="B57" s="4"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="13"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+      <c r="A59" s="13">
         <v>44699</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -1519,7 +1530,7 @@
       <c r="D62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1536,7 +1547,7 @@
       <c r="D63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="13"/>
+      <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
@@ -1551,7 +1562,7 @@
       <c r="D64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="13"/>
+      <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
@@ -1566,7 +1577,7 @@
       <c r="D65" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="13"/>
+      <c r="E65" s="12"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
@@ -1575,25 +1586,25 @@
       <c r="B66" s="4"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="13"/>
+      <c r="E66" s="12"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="11">
+      <c r="A68" s="13">
         <v>44699</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -1625,7 +1636,7 @@
       <c r="D71" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E71" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1642,7 +1653,7 @@
       <c r="D72" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="13"/>
+      <c r="E72" s="12"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
@@ -1657,7 +1668,7 @@
       <c r="D73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="13"/>
+      <c r="E73" s="12"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
@@ -1672,7 +1683,7 @@
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="13"/>
+      <c r="E74" s="12"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
@@ -1681,25 +1692,25 @@
       <c r="B75" s="4"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="13"/>
+      <c r="E75" s="12"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="11">
+      <c r="A77" s="13">
         <v>44699</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -1731,7 +1742,7 @@
       <c r="D80" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E80" s="13" t="s">
+      <c r="E80" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1748,7 +1759,7 @@
       <c r="D81" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="13"/>
+      <c r="E81" s="12"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
@@ -1763,7 +1774,7 @@
       <c r="D82" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E82" s="13"/>
+      <c r="E82" s="12"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
@@ -1778,7 +1789,7 @@
       <c r="D83" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="13"/>
+      <c r="E83" s="12"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
@@ -1793,7 +1804,7 @@
       <c r="D84" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E84" s="13"/>
+      <c r="E84" s="12"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
@@ -1802,25 +1813,25 @@
       <c r="B85" s="4"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="13"/>
+      <c r="E85" s="12"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="11">
+      <c r="A88" s="13">
         <v>44699</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
@@ -1852,7 +1863,7 @@
       <c r="D91" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E91" s="13" t="s">
+      <c r="E91" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1869,7 +1880,7 @@
       <c r="D92" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E92" s="13"/>
+      <c r="E92" s="12"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
@@ -1884,7 +1895,7 @@
       <c r="D93" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E93" s="13"/>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -1899,7 +1910,7 @@
       <c r="D94" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E94" s="13"/>
+      <c r="E94" s="12"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
@@ -1914,7 +1925,7 @@
       <c r="D95" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E95" s="13"/>
+      <c r="E95" s="12"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
@@ -1923,25 +1934,25 @@
       <c r="B96" s="4"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="13"/>
+      <c r="E96" s="12"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="11">
+      <c r="A98" s="13">
         <v>44699</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="12" t="s">
+      <c r="A99" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
@@ -1973,7 +1984,7 @@
       <c r="D101" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E101" s="13" t="s">
+      <c r="E101" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1990,7 +2001,7 @@
       <c r="D102" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E102" s="13"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
@@ -2005,14 +2016,14 @@
       <c r="D103" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E103" s="13"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>23</v>
@@ -2020,7 +2031,7 @@
       <c r="D104" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E104" s="13"/>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
@@ -2035,7 +2046,7 @@
       <c r="D105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="13"/>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
@@ -2044,35 +2055,137 @@
       <c r="B106" s="4"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="13"/>
+      <c r="E106" s="12"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="13">
+        <v>44730</v>
+      </c>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" s="12"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" s="12"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E114" s="12"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="E91:E96"/>
-    <mergeCell ref="E71:E75"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="E80:E85"/>
-    <mergeCell ref="A88:E88"/>
+  <mergeCells count="36">
+    <mergeCell ref="E111:E115"/>
+    <mergeCell ref="A98:E98"/>
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="E101:E106"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A109:E109"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="E13:E20"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="E4:E8"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="E13:E20"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E25:E30"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A98:E98"/>
-    <mergeCell ref="A99:E99"/>
-    <mergeCell ref="E101:E106"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="E35:E39"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="E44:E48"/>
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="E53:E57"/>
@@ -2081,6 +2194,13 @@
     <mergeCell ref="E62:E66"/>
     <mergeCell ref="A68:E68"/>
     <mergeCell ref="A69:E69"/>
+    <mergeCell ref="E71:E75"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="E80:E85"/>
+    <mergeCell ref="A88:E88"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="E91:E96"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{37B8BE8B-C1DE-46D5-ACA9-C62887FD6B84}"/>
@@ -2093,23 +2213,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c749dc0f-5474-4025-a529-a6cb3778208f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010019E651D14F13AF4EA865181F456D14A1" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="39f8623c144aa53429a9652546d11dc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bad4088f-bf3a-4720-9d78-c2bf33926734" xmlns:ns4="c749dc0f-5474-4025-a529-a6cb3778208f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7195bca6a4e2c96a9f52d7d2b36913c3" ns3:_="" ns4:_="">
     <xsd:import namespace="bad4088f-bf3a-4720-9d78-c2bf33926734"/>
@@ -2342,32 +2445,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5571F83D-2173-4796-B61B-148ABE77D105}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c749dc0f-5474-4025-a529-a6cb3778208f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bad4088f-bf3a-4720-9d78-c2bf33926734"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E4C579-54C9-439F-A962-2243282D7C86}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c749dc0f-5474-4025-a529-a6cb3778208f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0CF83AC-358A-4401-A76E-EB0DFCA9BD7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2384,4 +2479,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E4C579-54C9-439F-A962-2243282D7C86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5571F83D-2173-4796-B61B-148ABE77D105}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c749dc0f-5474-4025-a529-a6cb3778208f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bad4088f-bf3a-4720-9d78-c2bf33926734"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>